<commit_message>
* TestData.xlsx: * TestData (1).xlsx:
* TimeMaterialPage.cs: Made changes in the TM page
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="LoginPage" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="TimeAndMaterialPage" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Oiyo</t>
+  </si>
   <si>
     <t>Username</t>
   </si>
@@ -21,18 +34,31 @@
   <si>
     <t>hari</t>
   </si>
+  <si>
+    <t xml:space="preserve">This is a Data Driven Test </t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>This was edited</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -48,12 +74,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -67,7 +99,42 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123123.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -84,13 +151,30 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>123123.0</v>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>